<commit_message>
happy International Workers' Day！
</commit_message>
<xml_diff>
--- a/pop_of_S_28.xlsx
+++ b/pop_of_S_28.xlsx
@@ -1,26 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gyc\Desktop\fjyq_stat_model\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gyc\Desktop\fjyq_stat_model\fujian_stat_model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89554C1C-83FD-44BB-9DAB-EF2EAB3AB982}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B813B41A-28AB-4715-BD21-28D5863D99FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="19386" windowHeight="11733" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="58">
   <si>
     <t>age_cat7</t>
   </si>
@@ -68,6 +80,135 @@
   </si>
   <si>
     <t>at_most_partially</t>
+  </si>
+  <si>
+    <t>group</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>age1_vac1</t>
+  </si>
+  <si>
+    <t>age1_vac2</t>
+  </si>
+  <si>
+    <t>age1_vac3</t>
+  </si>
+  <si>
+    <t>age1_vac4</t>
+  </si>
+  <si>
+    <t>age2_vac1</t>
+  </si>
+  <si>
+    <t>age2_vac2</t>
+  </si>
+  <si>
+    <t>age2_vac3</t>
+  </si>
+  <si>
+    <t>age2_vac4</t>
+  </si>
+  <si>
+    <t>age3_vac1</t>
+  </si>
+  <si>
+    <t>age3_vac2</t>
+  </si>
+  <si>
+    <t>age3_vac3</t>
+  </si>
+  <si>
+    <t>age3_vac4</t>
+  </si>
+  <si>
+    <t>age4_vac1</t>
+  </si>
+  <si>
+    <t>age4_vac2</t>
+  </si>
+  <si>
+    <t>age4_vac3</t>
+  </si>
+  <si>
+    <t>age4_vac4</t>
+  </si>
+  <si>
+    <t>age5_vac1</t>
+  </si>
+  <si>
+    <t>age5_vac2</t>
+  </si>
+  <si>
+    <t>age5_vac3</t>
+  </si>
+  <si>
+    <t>age5_vac4</t>
+  </si>
+  <si>
+    <t>age6_vac1</t>
+  </si>
+  <si>
+    <t>age6_vac2</t>
+  </si>
+  <si>
+    <t>age6_vac3</t>
+  </si>
+  <si>
+    <t>age6_vac4</t>
+  </si>
+  <si>
+    <t>age7_vac1</t>
+  </si>
+  <si>
+    <t>age7_vac2</t>
+  </si>
+  <si>
+    <t>age7_vac3</t>
+  </si>
+  <si>
+    <t>age7_vac4</t>
+  </si>
+  <si>
+    <t>age1</t>
+  </si>
+  <si>
+    <t>vac1</t>
+  </si>
+  <si>
+    <t>vac2</t>
+  </si>
+  <si>
+    <t>vac3</t>
+  </si>
+  <si>
+    <t>vac4</t>
+  </si>
+  <si>
+    <t>age2</t>
+  </si>
+  <si>
+    <t>age3</t>
+  </si>
+  <si>
+    <t>age4</t>
+  </si>
+  <si>
+    <t>age5</t>
+  </si>
+  <si>
+    <t>age6</t>
+  </si>
+  <si>
+    <t>age7</t>
+  </si>
+  <si>
+    <t>age_group</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vac_group</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -422,18 +563,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="15.29296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="15.33203125" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -446,11 +588,20 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="H1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -463,44 +614,80 @@
       <c r="D2">
         <v>0.15252536514661599</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="H2">
         <v>6335917</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="H3" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="H4" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="H5" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -513,11 +700,20 @@
       <c r="D6">
         <v>0.10614338276285</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="H6">
         <v>4409205</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -530,11 +726,20 @@
       <c r="D7">
         <v>2.2299029992195298E-3</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="H7">
         <v>92630</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -547,11 +752,20 @@
       <c r="D8">
         <v>2.2299029992195298E-3</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="H8">
         <v>92630</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -564,11 +778,20 @@
       <c r="D9">
         <v>4.2368156985171102E-2</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="H9">
         <v>1759977</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -581,11 +804,20 @@
       <c r="D10">
         <v>2.47519232913368E-2</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="H10">
         <v>1028197</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -598,11 +830,20 @@
       <c r="D11">
         <v>6.3217750027873804E-2</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="H11">
         <v>2626071</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -615,11 +856,20 @@
       <c r="D12">
         <v>3.0661166239268602E-2</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="H12">
         <v>1273667</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -632,11 +882,20 @@
       <c r="D13">
         <v>1.4940350094770899E-2</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="H13">
         <v>620623</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -649,11 +908,20 @@
       <c r="D14">
         <v>2.97692050395808E-2</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="H14">
         <v>1236615</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -666,11 +934,20 @@
       <c r="D15">
         <v>0.132567733303601</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="H15">
         <v>5506875</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -683,11 +960,20 @@
       <c r="D16">
         <v>4.7162448433493098E-2</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="H16">
         <v>1959132</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>11</v>
       </c>
@@ -700,11 +986,20 @@
       <c r="D17">
         <v>2.7204816590478301E-2</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="H17">
         <v>1130090</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>12</v>
       </c>
@@ -717,11 +1012,20 @@
       <c r="D18">
         <v>1.4940350094770899E-2</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="H18">
         <v>620623</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -734,11 +1038,20 @@
       <c r="D19">
         <v>9.8450217415542399E-2</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="H19">
         <v>4089630</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>12</v>
       </c>
@@ -751,11 +1064,20 @@
       <c r="D20">
         <v>3.6458914037239401E-2</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="H20">
         <v>1514506</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>12</v>
       </c>
@@ -768,11 +1090,20 @@
       <c r="D21">
         <v>1.31564276953953E-2</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="H21">
         <v>546519</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>13</v>
       </c>
@@ -785,11 +1116,20 @@
       <c r="D22">
         <v>1.3044932545434301E-2</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="H22">
         <v>541888</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>13</v>
       </c>
@@ -802,11 +1142,20 @@
       <c r="D23">
         <v>6.0876351878693301E-2</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="H23">
         <v>2528809</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>13</v>
       </c>
@@ -819,11 +1168,20 @@
       <c r="D24">
         <v>2.4305942691492902E-2</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="H24">
         <v>1009671</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>13</v>
       </c>
@@ -836,11 +1194,20 @@
       <c r="D25">
         <v>1.33794179953172E-2</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="H25">
         <v>555782</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>14</v>
       </c>
@@ -853,11 +1220,20 @@
       <c r="D26">
         <v>1.6835767644107501E-2</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="H26">
         <v>699359</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>14</v>
       </c>
@@ -870,11 +1246,20 @@
       <c r="D27">
         <v>6.5782138476976303E-3</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="H27">
         <v>273260</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>14</v>
       </c>
@@ -887,11 +1272,20 @@
       <c r="D28">
         <v>1.18184858958635E-2</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="G28" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="H28">
         <v>490941</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>14</v>
       </c>
@@ -904,7 +1298,16 @@
       <c r="D29">
         <v>1.4382874344966001E-2</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F29" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="G29" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="H29">
         <v>597466</v>
       </c>
     </row>

</xml_diff>